<commit_message>
Updated Columnar output from SAS with better formats
</commit_message>
<xml_diff>
--- a/tika-parsers/src/test/resources/test-documents/test-columnar.xlsx
+++ b/tika-parsers/src/test/resources/test-documents/test-columnar.xlsx
@@ -10,9 +10,9 @@
     <sheet name="testing" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="testing">testing!$A$1:$H$12</definedName>
+    <definedName name="testing">'testing'!$A$1:$H$12</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -140,11 +140,272 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AAA1048576"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -203,10 +464,10 @@
         <v>21916</v>
       </c>
       <c r="G2" s="3">
-        <v>21916.0000116</v>
+        <v>21916.000011574073</v>
       </c>
       <c r="H2" s="2">
-        <v>0.0000116</v>
+        <v>1.1574074074074073e-05</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -220,7 +481,7 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>.1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -229,10 +490,10 @@
         <v>21917</v>
       </c>
       <c r="G3" s="3">
-        <v>21916.0001157</v>
+        <v>21916.000115740742</v>
       </c>
       <c r="H3" s="2">
-        <v>0.0000347</v>
+        <v>3.472222222222222e-05</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -246,19 +507,19 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>0.2</v>
+        <v>.2</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>.5</v>
       </c>
       <c r="F4" s="12">
         <v>21932</v>
       </c>
       <c r="G4" s="3">
-        <v>21916.0011574</v>
+        <v>21916.00115740741</v>
       </c>
       <c r="H4" s="2">
-        <v>0.0001042</v>
+        <v>.00010416666666666666</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -272,19 +533,19 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>0.3</v>
+        <v>.3</v>
       </c>
       <c r="E5">
-        <v>0.6666667</v>
+        <v>.6666666666666666</v>
       </c>
       <c r="F5" s="12">
         <v>21997</v>
       </c>
       <c r="G5" s="3">
-        <v>21916.0115741</v>
+        <v>21916.011574074077</v>
       </c>
       <c r="H5" s="2">
-        <v>0.0003125</v>
+        <v>.0003125</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -298,19 +559,19 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>0.4</v>
+        <v>.4</v>
       </c>
       <c r="E6">
-        <v>0.75</v>
+        <v>.75</v>
       </c>
       <c r="F6" s="12">
         <v>22172</v>
       </c>
       <c r="G6" s="3">
-        <v>21916.1157407</v>
+        <v>21916.11574074074</v>
       </c>
       <c r="H6" s="2">
-        <v>0.0009375</v>
+        <v>.0009375000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -324,19 +585,19 @@
         <v>13</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>.5</v>
       </c>
       <c r="E7">
-        <v>0.8</v>
+        <v>.8</v>
       </c>
       <c r="F7" s="12">
         <v>22541</v>
       </c>
       <c r="G7" s="3">
-        <v>21917.1574074</v>
+        <v>21917.15740740741</v>
       </c>
       <c r="H7" s="2">
-        <v>0.0028125</v>
+        <v>.0028125</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -350,19 +611,19 @@
         <v>14</v>
       </c>
       <c r="D8">
-        <v>0.6</v>
+        <v>.6</v>
       </c>
       <c r="E8">
-        <v>0.8333333</v>
+        <v>.8333333333333334</v>
       </c>
       <c r="F8" s="12">
         <v>23212</v>
       </c>
       <c r="G8" s="3">
-        <v>21927.5740741</v>
+        <v>21927.574074074077</v>
       </c>
       <c r="H8" s="2">
-        <v>0.0084375</v>
+        <v>.0084375</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -376,19 +637,19 @@
         <v>15</v>
       </c>
       <c r="D9">
-        <v>0.7</v>
+        <v>.7</v>
       </c>
       <c r="E9">
-        <v>0.8571429</v>
+        <v>.8571428571428571</v>
       </c>
       <c r="F9" s="12">
         <v>24317</v>
       </c>
       <c r="G9" s="3">
-        <v>22031.7407407</v>
+        <v>22031.74074074074</v>
       </c>
       <c r="H9" s="2">
-        <v>0.0253125</v>
+        <v>.0253125</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -402,19 +663,19 @@
         <v>16</v>
       </c>
       <c r="D10">
-        <v>0.8</v>
+        <v>.8</v>
       </c>
       <c r="E10">
-        <v>0.875</v>
+        <v>.875</v>
       </c>
       <c r="F10" s="12">
         <v>26012</v>
       </c>
       <c r="G10" s="3">
-        <v>23073.4074074</v>
+        <v>23073.40740740741</v>
       </c>
       <c r="H10" s="2">
-        <v>0.0759375</v>
+        <v>.07593749999999999</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -428,19 +689,19 @@
         <v>17</v>
       </c>
       <c r="D11">
-        <v>0.9</v>
+        <v>.9</v>
       </c>
       <c r="E11">
-        <v>0.8888889</v>
+        <v>.8888888888888888</v>
       </c>
       <c r="F11" s="12">
         <v>28477</v>
       </c>
       <c r="G11" s="3">
-        <v>33490.0740741</v>
+        <v>33490.07407407407</v>
       </c>
       <c r="H11" s="2">
-        <v>0.2278125</v>
+        <v>.2278125</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -457,16 +718,16 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0.9</v>
+        <v>.9</v>
       </c>
       <c r="F12" s="12">
         <v>31916</v>
       </c>
       <c r="G12" s="3">
-        <v>137656.7407407</v>
+        <v>137656.74074074073</v>
       </c>
       <c r="H12" s="2">
-        <v>0.6834375</v>
+        <v>.6834375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Formatted columns in the columnar test Excel files
</commit_message>
<xml_diff>
--- a/tika-parsers/src/test/resources/test-documents/test-columnar.xlsx
+++ b/tika-parsers/src/test/resources/test-documents/test-columnar.xlsx
@@ -10,9 +10,9 @@
     <sheet name="testing" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="testing">'testing'!$A$1:$H$12</definedName>
+    <definedName name="testing">testing!$A$1:$H$12</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="true"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -80,8 +80,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
+  <numFmts count="3">
+    <numFmt numFmtId="166" formatCode="[$-409]dd\-mm\-yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="ddmmmyy\ hh:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -112,20 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -151,39 +145,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,163 +256,185 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -431,19 +447,19 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -457,17 +473,17 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="2">
         <v>21916</v>
       </c>
       <c r="G2" s="3">
         <v>21916.000011574073</v>
       </c>
-      <c r="H2" s="2">
-        <v>1.1574074074074073e-05</v>
+      <c r="H2" s="4">
+        <v>1.1574074074074073E-5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -480,20 +496,20 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
-        <v>.1</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="2">
         <v>21917</v>
       </c>
       <c r="G3" s="3">
         <v>21916.000115740742</v>
       </c>
-      <c r="H3" s="2">
-        <v>3.472222222222222e-05</v>
+      <c r="H3" s="4">
+        <v>3.4722222222222222E-5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -506,20 +522,20 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4">
-        <v>.2</v>
-      </c>
-      <c r="E4">
-        <v>.5</v>
-      </c>
-      <c r="F4" s="12">
+      <c r="D4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="2">
         <v>21932</v>
       </c>
       <c r="G4" s="3">
-        <v>21916.00115740741</v>
-      </c>
-      <c r="H4" s="2">
-        <v>.00010416666666666666</v>
+        <v>21916.001157407409</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.0416666666666666E-4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -532,20 +548,20 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
-        <v>.3</v>
-      </c>
-      <c r="E5">
-        <v>.6666666666666666</v>
-      </c>
-      <c r="F5" s="12">
+      <c r="D5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F5" s="2">
         <v>21997</v>
       </c>
       <c r="G5" s="3">
         <v>21916.011574074077</v>
       </c>
-      <c r="H5" s="2">
-        <v>.0003125</v>
+      <c r="H5" s="4">
+        <v>3.1250000000000001E-4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -558,20 +574,20 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6">
-        <v>.4</v>
-      </c>
-      <c r="E6">
-        <v>.75</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="D6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F6" s="2">
         <v>22172</v>
       </c>
       <c r="G6" s="3">
-        <v>21916.11574074074</v>
-      </c>
-      <c r="H6" s="2">
-        <v>.0009375000000000001</v>
+        <v>21916.115740740741</v>
+      </c>
+      <c r="H6" s="4">
+        <v>9.3750000000000007E-4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -584,20 +600,20 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
-        <v>.5</v>
-      </c>
-      <c r="E7">
-        <v>.8</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="D7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="2">
         <v>22541</v>
       </c>
       <c r="G7" s="3">
-        <v>21917.15740740741</v>
-      </c>
-      <c r="H7" s="2">
-        <v>.0028125</v>
+        <v>21917.157407407409</v>
+      </c>
+      <c r="H7" s="4">
+        <v>2.8124999999999999E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -610,20 +626,20 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8">
-        <v>.6</v>
-      </c>
-      <c r="E8">
-        <v>.8333333333333334</v>
-      </c>
-      <c r="F8" s="12">
+      <c r="D8" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F8" s="2">
         <v>23212</v>
       </c>
       <c r="G8" s="3">
         <v>21927.574074074077</v>
       </c>
-      <c r="H8" s="2">
-        <v>.0084375</v>
+      <c r="H8" s="4">
+        <v>8.4375000000000006E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -636,20 +652,20 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9">
-        <v>.7</v>
-      </c>
-      <c r="E9">
-        <v>.8571428571428571</v>
-      </c>
-      <c r="F9" s="12">
+      <c r="D9" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="F9" s="2">
         <v>24317</v>
       </c>
       <c r="G9" s="3">
-        <v>22031.74074074074</v>
-      </c>
-      <c r="H9" s="2">
-        <v>.0253125</v>
+        <v>22031.740740740741</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2.5312500000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -662,20 +678,20 @@
       <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D10">
-        <v>.8</v>
-      </c>
-      <c r="E10">
-        <v>.875</v>
-      </c>
-      <c r="F10" s="12">
+      <c r="D10" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F10" s="2">
         <v>26012</v>
       </c>
       <c r="G10" s="3">
-        <v>23073.40740740741</v>
-      </c>
-      <c r="H10" s="2">
-        <v>.07593749999999999</v>
+        <v>23073.407407407409</v>
+      </c>
+      <c r="H10" s="4">
+        <v>7.5937499999999991E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -688,20 +704,20 @@
       <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="D11">
-        <v>.9</v>
-      </c>
-      <c r="E11">
-        <v>.8888888888888888</v>
-      </c>
-      <c r="F11" s="12">
+      <c r="D11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F11" s="2">
         <v>28477</v>
       </c>
       <c r="G11" s="3">
-        <v>33490.07407407407</v>
-      </c>
-      <c r="H11" s="2">
-        <v>.2278125</v>
+        <v>33490.074074074073</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.2278125</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -714,24 +730,25 @@
       <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>.9</v>
-      </c>
-      <c r="F12" s="12">
+      <c r="E12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="F12" s="2">
         <v>31916</v>
       </c>
       <c r="G12" s="3">
         <v>137656.74074074073</v>
       </c>
-      <c r="H12" s="2">
-        <v>.6834375</v>
+      <c r="H12" s="4">
+        <v>0.68343750000000003</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>